<commit_message>
Update jscoresdk test case to temporary remove 2 block case
</commit_message>
<xml_diff>
--- a/autotest/client/jscoresdk/data/pluraldata.xlsx
+++ b/autotest/client/jscoresdk/data/pluraldata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junw\OneDrive - VMware, Inc\VMwareCorp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junw\AppData\Local\Temp\BvSshSftp\Bv001c4b\Bv0024d6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{44815440-3CA3-40C4-B1B5-3D8C5B5156C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AE020C10-4AAE-4A6F-93B1-CB7D19DC2FED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78442B5-5148-4537-A2BA-1ACFA086BD72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="1680" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="343">
   <si>
     <t>Function</t>
   </si>
@@ -2292,7 +2292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2325,6 +2325,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2604,7 +2610,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2859,8 +2865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="A276" sqref="A276:XFD276"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298:XFD298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8676,27 +8682,51 @@
       <c r="H274" s="6"/>
       <c r="I274" s="6"/>
     </row>
-    <row r="275" spans="1:10">
-      <c r="A275" s="6"/>
-      <c r="B275" s="6"/>
-      <c r="C275" s="6"/>
-      <c r="D275" s="6"/>
-      <c r="E275" s="6"/>
-      <c r="F275" s="6"/>
-      <c r="G275" s="6"/>
-      <c r="H275" s="6"/>
-      <c r="I275" s="6"/>
-    </row>
-    <row r="276" spans="1:10">
-      <c r="A276" s="6"/>
-      <c r="B276" s="6"/>
-      <c r="C276" s="6"/>
-      <c r="D276" s="6"/>
-      <c r="E276" s="6"/>
-      <c r="F276" s="6"/>
-      <c r="G276" s="6"/>
-      <c r="H276" s="6"/>
-      <c r="I276" s="6"/>
+    <row r="275" spans="1:10" s="12" customFormat="1">
+      <c r="A275" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B275" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C275" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D275" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E275" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F275" s="11"/>
+      <c r="G275" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="H275" s="11"/>
+      <c r="I275" s="11"/>
+    </row>
+    <row r="276" spans="1:10" s="12" customFormat="1">
+      <c r="A276" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B276" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C276" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D276" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E276" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F276" s="11"/>
+      <c r="G276" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="H276" s="11"/>
+      <c r="I276" s="11"/>
     </row>
     <row r="277" spans="1:10">
       <c r="A277" s="6"/>
@@ -9201,52 +9231,24 @@
       <c r="I296" s="6"/>
     </row>
     <row r="297" spans="1:9">
-      <c r="A297" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B297" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C297" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D297" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E297" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F297" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G297" s="6" t="s">
-        <v>224</v>
-      </c>
+      <c r="A297" s="6"/>
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
+      <c r="D297" s="6"/>
+      <c r="E297" s="6"/>
+      <c r="F297" s="6"/>
+      <c r="G297" s="6"/>
       <c r="H297" s="6"/>
       <c r="I297" s="6"/>
     </row>
     <row r="298" spans="1:9">
-      <c r="A298" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B298" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C298" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D298" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E298" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F298" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G298" s="6" t="s">
-        <v>224</v>
-      </c>
+      <c r="A298" s="6"/>
+      <c r="B298" s="6"/>
+      <c r="C298" s="6"/>
+      <c r="D298" s="6"/>
+      <c r="E298" s="6"/>
+      <c r="F298" s="6"/>
+      <c r="G298" s="6"/>
       <c r="H298" s="6"/>
       <c r="I298" s="6"/>
     </row>

</xml_diff>